<commit_message>
Add picture option to kindergarten dish
</commit_message>
<xml_diff>
--- a/xlsforms/kindergartendish.xlsx
+++ b/xlsforms/kindergartendish.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -51,35 +51,7 @@
     <t xml:space="preserve">Kindergarten</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">wq:ForeignKey("institution.I</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">nstitution</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">")</t>
-    </r>
+    <t xml:space="preserve">wq:ForeignKey("kindergarten.Kindergarten")</t>
   </si>
   <si>
     <t xml:space="preserve">date</t>
@@ -101,6 +73,15 @@
   </si>
   <si>
     <t xml:space="preserve">Please enter the name of the ingredients separated by a comma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">image</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Picture of the dish</t>
   </si>
   <si>
     <t xml:space="preserve">note</t>
@@ -245,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -299,12 +280,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -439,7 +414,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -451,7 +426,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -532,10 +507,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ35"/>
+  <dimension ref="A1:AMJ36"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -571,7 +546,7 @@
       <c r="AMI1" s="7"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="12" customFormat="true" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="12" customFormat="true" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
@@ -628,40 +603,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G6" s="4"/>
-      <c r="AMJ6" s="0"/>
-    </row>
-    <row r="7" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="B6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
+      <c r="C6" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G7" s="4"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="14" t="s">
+      <c r="A8" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="B8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="D8" s="0"/>
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
-        <v>6</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>23</v>
@@ -669,19 +641,21 @@
       <c r="C9" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="E10" s="9" t="s">
         <v>28</v>
       </c>
       <c r="F10" s="15"/>
@@ -700,19 +674,19 @@
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B12" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="15"/>
+    </row>
+    <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>35</v>
@@ -722,7 +696,7 @@
       </c>
       <c r="F13" s="15"/>
     </row>
-    <row r="14" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
         <v>37</v>
       </c>
@@ -734,37 +708,48 @@
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="13"/>
+      <c r="B15" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>42</v>
+      </c>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G16" s="4"/>
-      <c r="AMJ16" s="0"/>
-    </row>
-    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="13"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G17" s="4"/>
+      <c r="AMJ17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -799,6 +784,7 @@
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -832,7 +818,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -843,68 +829,68 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -953,28 +939,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D2" s="19" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
Update kindergarten dish (remove/rearrange fields and add type)
</commit_message>
<xml_diff>
--- a/xlsforms/kindergartendish.xlsx
+++ b/xlsforms/kindergartendish.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="67">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -63,16 +63,37 @@
     <t xml:space="preserve">Enter the name of the dish</t>
   </si>
   <si>
-    <t xml:space="preserve">text</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ingredient_list</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ingredients</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please enter the name of the ingredients separated by a comma.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">select_one </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">meal_type</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of meal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">select_one waste_choices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">waste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Food waste – how much of the dish you have to dump into the garbage?</t>
   </si>
   <si>
     <t xml:space="preserve">image</t>
@@ -111,15 +132,6 @@
     <t xml:space="preserve">wq:ForeignKey("ingredient.Ingredient")</t>
   </si>
   <si>
-    <t xml:space="preserve">integer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quantity_pieces</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enter the quantity of the ingredient (pieces)</t>
-  </si>
-  <si>
     <t xml:space="preserve">decimal</t>
   </si>
   <si>
@@ -132,7 +144,7 @@
     <t xml:space="preserve">calories</t>
   </si>
   <si>
-    <t xml:space="preserve">Enter the number of calories per ingredient in the dish (calories)</t>
+    <t xml:space="preserve">Enter the number of calories of the ingredient</t>
   </si>
   <si>
     <t xml:space="preserve">select_one from_producer_choices</t>
@@ -144,15 +156,6 @@
     <t xml:space="preserve">Was the ingredient bought directly from the producer?</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one waste_choices</t>
-  </si>
-  <si>
-    <t xml:space="preserve">waste</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Food waste – how many of the dish you have to dump into the garbage?</t>
-  </si>
-  <si>
     <t xml:space="preserve">end repeat</t>
   </si>
   <si>
@@ -199,6 +202,27 @@
   </si>
   <si>
     <t xml:space="preserve">More than 75 %</t>
+  </si>
+  <si>
+    <t xml:space="preserve">meal_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">breakfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breakfast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">afternoon_tea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afternoon tea</t>
   </si>
   <si>
     <t xml:space="preserve">form_title</t>
@@ -226,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -280,6 +304,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
@@ -414,7 +444,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -426,7 +456,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -507,10 +537,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ36"/>
+  <dimension ref="A1:AMJ35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -594,162 +624,147 @@
         <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="1" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="9" t="s">
+      <c r="C6" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G7" s="4"/>
-      <c r="AMJ7" s="0"/>
-    </row>
-    <row r="8" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="0" t="s">
+    </row>
+    <row r="8" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G8" s="4"/>
+      <c r="AMJ8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-    </row>
-    <row r="9" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="D9" s="0"/>
+      <c r="E9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="C10" s="13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13" t="s">
+      <c r="E10" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="C11" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13" t="s">
+      <c r="E11" s="9" t="s">
         <v>29</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>31</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>32</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>34</v>
       </c>
       <c r="F12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="15"/>
-    </row>
-    <row r="15" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>42</v>
-      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="13"/>
       <c r="F15" s="15"/>
     </row>
-    <row r="16" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="13"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="G17" s="4"/>
-      <c r="AMJ17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="25" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="26" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="16" s="7" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G16" s="4"/>
+      <c r="AMJ16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="22" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="23" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="40.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="25" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="26" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="28" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="28" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="31" customFormat="false" ht="36.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="32" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="31" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="38.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -784,7 +799,6 @@
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -804,7 +818,7 @@
   <dimension ref="A1:C1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -818,7 +832,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B1" s="17" t="s">
         <v>1</v>
@@ -829,71 +843,103 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -939,28 +985,28 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="17" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C1" s="17" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D1" s="18" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" s="19" t="n">
         <v>1</v>

</xml_diff>